<commit_message>
setting postgres version to 13
</commit_message>
<xml_diff>
--- a/output/prediction.xlsx
+++ b/output/prediction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>Reason</t>
   </si>
@@ -64,10 +64,10 @@
     <t>Gynae.</t>
   </si>
   <si>
+    <t>Developmental / Behavioural</t>
+  </si>
+  <si>
     <t>x ray request</t>
-  </si>
-  <si>
-    <t>Developmental / Behavioural</t>
   </si>
   <si>
     <t>non pain</t>
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -421,9 +421,10 @@
     <col min="12" max="12" width="40.7109375" customWidth="1"/>
     <col min="13" max="13" width="40.7109375" customWidth="1"/>
     <col min="14" max="14" width="40.7109375" customWidth="1"/>
+    <col min="15" max="15" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +467,11 @@
       <c r="N1" t="s">
         <v>2</v>
       </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -510,25 +514,28 @@
       <c r="N2" t="s">
         <v>15</v>
       </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -537,6 +544,9 @@
       </c>
       <c r="C4" t="s">
         <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>